<commit_message>
Update Boyer Probate Tracking.xlsx
</commit_message>
<xml_diff>
--- a/Boyer Probate Tracking.xlsx
+++ b/Boyer Probate Tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emilyboyer/Desktop/signed sealed delivered/Signed-Sealed-Delivered/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{607EB1D2-3693-4246-B222-4E60A4CD3723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E0F1122-DE25-BB43-9118-3ADACF90C35A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13460" yWindow="500" windowWidth="22380" windowHeight="20420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="149">
   <si>
     <t xml:space="preserve">Source: </t>
   </si>
@@ -466,6 +466,9 @@
   <si>
     <t>MD_CC_PRO_063_1677_8_King</t>
   </si>
+  <si>
+    <t>MD_CC_PRO_064_1678_Douglass</t>
+  </si>
 </sst>
 </file>
 
@@ -585,7 +588,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -811,7 +814,7 @@
   <dimension ref="A1:X1001"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A30" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -2441,135 +2444,135 @@
       <c r="W37" s="1"/>
       <c r="X37" s="1"/>
     </row>
-    <row r="38" spans="1:24" s="21" customFormat="1" ht="16">
-      <c r="A38" s="17" t="s">
+    <row r="38" spans="1:24" ht="16">
+      <c r="A38" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="B38" s="18" t="s">
+      <c r="B38" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C38" s="18" t="s">
+      <c r="C38" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="D38" s="18" t="s">
+      <c r="D38" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E38" s="19" t="s">
+      <c r="E38" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="F38" s="20" t="s">
+      <c r="F38" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G38" s="18" t="s">
+      <c r="G38" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H38" s="18" t="s">
+      <c r="H38" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I38" s="18"/>
-      <c r="J38" s="18" t="s">
+      <c r="I38" s="1"/>
+      <c r="J38" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="K38" s="18"/>
-      <c r="L38" s="18"/>
-      <c r="M38" s="18"/>
-      <c r="N38" s="18"/>
-      <c r="O38" s="18"/>
-      <c r="P38" s="18"/>
-      <c r="Q38" s="18"/>
-      <c r="R38" s="18"/>
-      <c r="S38" s="18"/>
-      <c r="T38" s="18"/>
-      <c r="U38" s="18"/>
-      <c r="V38" s="18"/>
-      <c r="W38" s="18"/>
-      <c r="X38" s="18"/>
-    </row>
-    <row r="39" spans="1:24" s="21" customFormat="1" ht="16">
-      <c r="A39" s="17" t="s">
+      <c r="K38" s="1"/>
+      <c r="L38" s="1"/>
+      <c r="M38" s="1"/>
+      <c r="N38" s="1"/>
+      <c r="O38" s="1"/>
+      <c r="P38" s="1"/>
+      <c r="Q38" s="1"/>
+      <c r="R38" s="1"/>
+      <c r="S38" s="1"/>
+      <c r="T38" s="1"/>
+      <c r="U38" s="1"/>
+      <c r="V38" s="1"/>
+      <c r="W38" s="1"/>
+      <c r="X38" s="1"/>
+    </row>
+    <row r="39" spans="1:24" ht="16">
+      <c r="A39" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="B39" s="18" t="s">
+      <c r="B39" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C39" s="18" t="s">
+      <c r="C39" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D39" s="18" t="s">
+      <c r="D39" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E39" s="19" t="s">
+      <c r="E39" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="F39" s="20" t="s">
+      <c r="F39" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G39" s="18" t="s">
+      <c r="G39" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H39" s="18" t="s">
+      <c r="H39" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I39" s="18"/>
-      <c r="J39" s="18" t="s">
+      <c r="I39" s="1"/>
+      <c r="J39" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="K39" s="18"/>
-      <c r="L39" s="18"/>
-      <c r="M39" s="18"/>
-      <c r="N39" s="18"/>
-      <c r="O39" s="18"/>
-      <c r="P39" s="18"/>
-      <c r="Q39" s="18"/>
-      <c r="R39" s="18"/>
-      <c r="S39" s="18"/>
-      <c r="T39" s="18"/>
-      <c r="U39" s="18"/>
-      <c r="V39" s="18"/>
-      <c r="W39" s="18"/>
-      <c r="X39" s="18"/>
-    </row>
-    <row r="40" spans="1:24" s="14" customFormat="1" ht="16">
-      <c r="A40" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="B40" s="11" t="s">
+      <c r="K39" s="1"/>
+      <c r="L39" s="1"/>
+      <c r="M39" s="1"/>
+      <c r="N39" s="1"/>
+      <c r="O39" s="1"/>
+      <c r="P39" s="1"/>
+      <c r="Q39" s="1"/>
+      <c r="R39" s="1"/>
+      <c r="S39" s="1"/>
+      <c r="T39" s="1"/>
+      <c r="U39" s="1"/>
+      <c r="V39" s="1"/>
+      <c r="W39" s="1"/>
+      <c r="X39" s="1"/>
+    </row>
+    <row r="40" spans="1:24" s="21" customFormat="1" ht="16">
+      <c r="A40" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="B40" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C40" s="11" t="s">
+      <c r="C40" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="D40" s="11" t="s">
+      <c r="D40" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E40" s="15">
+      <c r="E40" s="19">
         <v>1678</v>
       </c>
-      <c r="F40" s="12" t="s">
+      <c r="F40" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="G40" s="13" t="s">
+      <c r="G40" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="H40" s="11" t="s">
+      <c r="H40" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="I40" s="11"/>
-      <c r="J40" s="11"/>
-      <c r="K40" s="11"/>
-      <c r="L40" s="11"/>
-      <c r="M40" s="11"/>
-      <c r="N40" s="11"/>
-      <c r="O40" s="11"/>
-      <c r="P40" s="11"/>
-      <c r="Q40" s="11"/>
-      <c r="R40" s="11"/>
-      <c r="S40" s="11"/>
-      <c r="T40" s="11"/>
-      <c r="U40" s="11"/>
-      <c r="V40" s="11"/>
-      <c r="W40" s="11"/>
-      <c r="X40" s="11"/>
+      <c r="I40" s="18"/>
+      <c r="J40" s="18"/>
+      <c r="K40" s="18"/>
+      <c r="L40" s="18"/>
+      <c r="M40" s="18"/>
+      <c r="N40" s="18"/>
+      <c r="O40" s="18"/>
+      <c r="P40" s="18"/>
+      <c r="Q40" s="18"/>
+      <c r="R40" s="18"/>
+      <c r="S40" s="18"/>
+      <c r="T40" s="18"/>
+      <c r="U40" s="18"/>
+      <c r="V40" s="18"/>
+      <c r="W40" s="18"/>
+      <c r="X40" s="18"/>
     </row>
     <row r="41" spans="1:24" s="14" customFormat="1" ht="16">
       <c r="A41" s="10" t="s">

</xml_diff>